<commit_message>
Fixed annotation in example data
</commit_message>
<xml_diff>
--- a/Examples/SR1_July2011_calibr_plain.xlsx
+++ b/Examples/SR1_July2011_calibr_plain.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="120">
   <si>
     <t>id</t>
   </si>
@@ -372,6 +372,9 @@
   <si>
     <t>Non-transgenic line, growth</t>
   </si>
+  <si>
+    <t>BZ</t>
+  </si>
 </sst>
 </file>
 
@@ -713,7 +716,7 @@
   <dimension ref="A1:IL99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -63584,7 +63587,7 @@
         <v>12</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H88" s="3">
         <v>10</v>
@@ -64306,7 +64309,7 @@
         <v>12</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H89" s="3">
         <v>10</v>
@@ -65028,7 +65031,7 @@
         <v>12</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H90" s="3">
         <v>10</v>
@@ -65750,7 +65753,7 @@
         <v>12</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H91" s="3">
         <v>10</v>
@@ -66472,7 +66475,7 @@
         <v>12</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H92" s="3">
         <v>10</v>
@@ -72230,7 +72233,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>